<commit_message>
fixed item 29 title.
</commit_message>
<xml_diff>
--- a/Effective Modern C++ Things to Remember.xlsx
+++ b/Effective Modern C++ Things to Remember.xlsx
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,15 +1093,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:4" s="3" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+    <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="17" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1113,6 +1109,10 @@
       <c r="D45" s="6" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="46" spans="2:4" s="3" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
@@ -1243,7 +1243,7 @@
     <brk id="12" max="16383" man="1"/>
     <brk id="24" max="16383" man="1"/>
     <brk id="33" max="16383" man="1"/>
-    <brk id="45" max="16383" man="1"/>
+    <brk id="42" max="16383" man="1"/>
     <brk id="57" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>

</xml_diff>